<commit_message>
llama2_general.py is a more general llama2 class that has memory; updated automatic prompt engineering workflow
</commit_message>
<xml_diff>
--- a/test/prompt_engineering_comparison.xlsx
+++ b/test/prompt_engineering_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianyuyang/Desktop/CMU MSCF Courses/Mini 5/ML_Capstone/QACapstone/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965BD5E4-BDB2-274B-A147-C8A65C7BDF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191B6D93-44C3-1747-BDCA-613420F0574B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,32 +42,34 @@
   <si>
     <t>MID-YEAR OUTLOOK 2024
 OUTLOOK 2024  KEY THEMES  Macroeconomy:  A Longer Path to Normalization    Geopolitics and Elections:  Roadmaps for Resilience  Tailwinds and Headwinds:   Investing in Megatrends
-This financial promotion is provided by Goldman Sachs Asset Management B.V.</t>
+This financial promotion is provided by Goldman Sachs Asset Management B.V.
+query_resposne_sim:0.8554397494584152</t>
   </si>
   <si>
     <t>3. Goldman Sachs Asset Management, Company Information. As of June, 2024.
 4. Goldman Sachs Asset Management. As of December 29, 2023. Past performance does not guarantee future results, which may vary.
 Tokyo Stock Exchange, Goldman Sachs Global
-query_response_sim:0.7584750633787378</t>
+query_response_sim: 0.7584750633787378</t>
   </si>
   <si>
     <t>llama2</t>
   </si>
   <si>
-    <t>Based on the provided context, the key takeaway of Goldman Sachs' mid-year outlook for 2024 is that the economic realities are taking shape, including higher-for-longer interest rates, elevated geopolitical risk, and megatrends rapidly transforming industries. The report highlights the need for a dynamic investment approach in the months ahead as the macroeconomic cycle adjusts, and emphasizes the importance of understanding the nuances of these forces and how they interconnect to potentially capitalize on the opportunities they create.</t>
-  </si>
-  <si>
-    <t>Based on the provided context information, the key takeaway of Goldman Sachs' mid-year outlook 2024 is that the firm expects a global economic slowdown in the near term, with potential risks to growth and stability. The section titles from GS indicate that they have provided insights on various aspects of the economy, including inflation, interest rates, currencies, and commodities.
+    <t>Based on the provided context information, the key takeaway of Goldman's mid-year outlook 2024 is that the firm believes that new economic realities are taking shape, including higher-for-longer interest rates, elevated geopolitical risk, and megatrends rapidly transforming industries. They also highlight the need for a dynamic investment approach in the months ahead as the macroeconomic cycle adjusts, and note that understanding the nuances of these forces and how they interconnect can enable companies and investors to potentially capitalize on the opportunities they create.
+query_resposne_sim:0.8871544712301357</t>
+  </si>
+  <si>
+    <t>Based on the provided context information, the key takeaway of Goldman Sachs' mid-year outlook 2024 is that they expect a global economic recovery to continue in 2024, with improved prospects for growth and inflation. The report highlights several factors contributing to this outlook, including:
+1. Improved economic data: Goldman Sachs notes that recent economic data has shown signs of improvement, including a rebound in global trade, increased consumer confidence, and a pickup in business investment.
+2. Central bank support: The report emphasizes the role of central banks in supporting the recovery, particularly through monetary policy accommodation and liquidity provision.
+3. Fiscal stimulus: Goldman Sachs highlights the potential for fiscal stimulus to contribute to growth, particularly in countries with more flexible fiscal policies.
+4. Improved corporate earnings: The report notes that corporate earnings have shown signs of improvement, with many companies reporting higher profits and revenues.
 Relevant numbers given in the report include:
-* Detection class probability of 0.5797362923622131 for the document as a whole, indicating a moderate level of confidence in the analysis.
-* Coordinates for two sets of points, indicating the location of the data on a PixelSpace layout with a width of 2200 and a height of 1700.
-* Last modified date of 2024-09-30T10:17:23, indicating that the report was updated recently.
-* Filetype of application/pdf, indicating that the report is in PDF format.
-* Languages listed as ['eng'], indicating that the report is written in English.
-* Page number of 8 and 25, indicating the location of two key sections within the report.
-* Filename of fi-outlook_3q24.pdf, indicating the specific name of the report.
-Overall, Goldman Sachs' mid-year outlook 2024 suggests that the global economy may face challenges in the near term, but also highlights potential opportunities for growth and investment.
-query_response_sim:0.8444316485839105</t>
+1. Global economic growth forecast: Goldman Sachs is forecasting a pickup in global economic growth to 3.9% in 2024, up from 3.5% in 2023.
+2. Inflation forecast: The report predicts that inflation will rise to 1.8% in 2024, up from 1.5% in 2023, driven by improving economic growth and higher commodity prices.
+3. Interest rate expectations: Goldman Sachs expects short-term interest rates to rise gradually over the next year, with the federal funds rate expected to reach 2.75% by the end of 2024.
+4. Stock market performance: The report notes that equity markets have performed well in recent months, with the S&amp;P 500 index up 13% since the start of the year.
+query_response_sim: 0.8374304368286721</t>
   </si>
   <si>
     <t>llamaparse</t>
@@ -79,7 +81,8 @@
 # Three Key Questions
 # 1
 Are investment theses predicated on the continuation of existing policies?
-Our View: While prudent investments are never predicated on a single factor, many investors are contemplating how potential policy removals, additions, or alterations can change underwriting assumptions. This can potentially be easier to navigate in the US, where many policies related to supply chains and energy resources have a bottom-up nature that target specific markets, as opposed to in Europe where top-down regulations can fundamentally change the landscape.</t>
+Our View: While prudent investments are never predicated on a single factor, many investors are contemplating how potential policy removals, additions, or alterations can change underwriting assumptions. This can potentially be easier to navigate in the US, where many policies related to supply chains and energy resources have a bottom-up nature that target specific markets, as opposed to in Europe where top-down regulations can fundamentally change the landscape.
+query_resposne_sim:0.8619108861396854</t>
   </si>
   <si>
     <t>Goldman Sachs Asset Management
@@ -87,45 +90,25 @@
 # TAILWINDS AND HEADWINDS:
 # INVESTING IN MEGATRENDS
 Beyond the near-term path of inflation, rates, and election results, we remain focused on longer-term paradigm shifts, including five key structural forces: decarbonization, digitization, deglobalization, destabilization in geopolitics, and demographic aging. Active investment strategies, a focus on diversification and risk management may become increasingly important to help navigate these contours and deliver alpha. Investors who stay in their silos and focus on a single theme may miss out on opportunities and underestimate risks.
-query_response_sim:0.791577934872893</t>
-  </si>
-  <si>
-    <t>The key takeaway of Goldman's mid-year outlook 2024 is that the macroeconomy is on a longer path to normalization, with considerable but still incomplete disinflation progress lengthening the path to interest rate normalization. This condition calls for active and dynamic investment strategies, and balanced allocations and hedging strategies can potentially add resilience to portfolios amid unstable geopolitics and election-related uncertainty. Additionally, areas of potential opportunity include core fixed income, equity exposures beyond the largest mega-cap names, and private market strategies focused on driving value creation at portfolio companies.</t>
-  </si>
-  <si>
-    <t>Based on the context information provided, the key takeaway of Goldman Sachs' Mid-Year Outlook 2024 is that the macroeconomy is on a longer path to normalization, with geopolitics and elections playing a significant role in shaping the investment landscape. The report highlights several key themes, including:
-1. Macroeconomy: Goldman Sachs expects the global economy to continue growing, but at a slower pace than previously expected. They predict that the US Federal Reserve will keep interest rates low for an extended period, and that inflation will remain subdued.
-2. Geopolitics and Elections: The report notes that geopolitical tensions and upcoming elections in various countries will continue to impact markets. Goldman Sachs expects these factors to create volatility and uncertainty, but also opportunities for investment in resilience.
-3. Tailwinds and Headwinds: The report identifies several megatrends that are expected to drive investment performance, including the growth of digital technologies, the rise of emerging markets, and the increasing importance of sustainability.
-Relevant numbers provided in the report include:
-1. US Bureau of Labor Statistics: As of June 12, 2024, the unemployment rate in the US is 3.6%, down from 3.8% in December 2023.
-2. European Central Bank: As of June 6, 2024, inflation in the Eurozone is at 1.7%, down from 2.1% in December 2023.
-3. Goldman Sachs Asset Management: As of December 29, 2023, the firm's equity strategies were overweight in technology, healthcare, and consumer discretionary stocks, and underweight in financials and real estate.
-4. Tokyo Stock Exchange: As of May 16, 2024, the Nikkei 225 index is at 23,584, up from 22,795 in December 2023.
-5. Goldman Sachs Global Investment Research: As of May 29, 2024, the firm's global economic growth forecast for 2024 is 3.6%, down from 3.8% in December 2023.
-6. Climate Bonds Initiative: As of June 20, 2024, the total value of green bonds issued globally is $175 billion, up from $129 billion in December 2023.
-query_response_sim:0.8282103345454851</t>
+query_response_sim: 0.791577934872893</t>
+  </si>
+  <si>
+    <t>The key takeaway of Goldman's mid-year outlook 2024 is that there is a longer path to interest rate normalization due to considerable but still incomplete disinflation progress, and active and dynamic investment strategies are needed to navigate the unstable geopolitics and election-related uncertainty.
+query_resposne_sim:0.8440195730301284</t>
+  </si>
+  <si>
+    <t>Based on the section titles provided in the context, the key takeaway of Goldman Sachs' mid-year outlook 2024 is that the macroeconomy is on a longer path to normalization, with geopolitics and elections playing a significant role in resilience. The report highlights tailwinds and headwinds in investing in megatrends, including the impact of climate change on the economy.
+Some relevant numbers provided in the report include:
+1. US Bureau of Labor Statistics: As of June 12, 2024, the unemployment rate stood at 3.6%, down from 3.8% in December 2023.
+2. European Central Bank: As of June 6, 2024, inflation rate in the Eurozone was 2.2%, down from 2.5% in December 2023.
+3. Goldman Sachs Asset Management: As of June 2024, the firm's assets under management stood at $1.6 trillion, up from $1.4 trillion in December 2023.
+4. Tokyo Stock Exchange: As of May 16, 2024, the Nikkei 225 index was trading at 22,798, down from 23,291 in December 2023.
+5. Climate Bonds Initiative: As of June 20, 2024, the global green bond market stood at $1.3 trillion, up from $1.2 trillion in December 2023.
+These numbers provide a general overview of the current state of the economy and financial markets, which can help inform investment decisions. However, it's important to note that past performance does not guarantee future results, and investors should always consult with their financial advisors before making any investment decisions.
+query_response_sim: 0.7886789955165893</t>
   </si>
   <si>
     <t>pdfplumber</t>
-  </si>
-  <si>
-    <t>Goldman Sachs Asset Management Asset Management Outlook 2024 | 18
-and Goldman Sachs Asset Management has no obligation to provide any maintain any licenses, authorizations or registrations in Asia (other
-updates or changes. than Japan), except that it conducts businesses (subject to applicable
-Views and opinions expressed are for informational purposes only local regulations) in and from the following jurisdictions: Hong Kong,
-and do not constitute a recommendation by Goldman Sachs Asset Singapore, India and China. This material has been issued for use in or
-Management to buy, sell, or hold any security. Views and opinions are from Hong Kong by Goldman Sachs Asset Management (Hong Kong)
-current as of the date of this presentation and may be subject to change, Limited and in or from Singapore by Goldman Sachs Asset Management
-they should not be construed as investment advice. (Singapore) Pte. Ltd. (Company Number: 201329851H).
-Individual portfolio management teams for Goldman Sachs Asset Australia and New Zealand: This material is distributed in Australia
-Management may have views and opinions and/or make investment and New Zealand by Goldman Sachs Asset Management Australia Pty
-decisions that, in certain instances, may not always be consistent with Ltd ABN 41 006 099 681, AFSL 228948 (’GSAMA’) and is intended
-the views and opinions expressed herein. for viewing only by wholesale clients in Australia for the purposes of
-section 761G of the Corporations Act 2001 (Cth) and to clients who
-The website links provided are for your convenience only and are not an either fall within any or all of the categories of investors set out in
-endorsement or recommendation by Goldman Sachs Asset Management section 3(2) or sub-section 5(2CC) of the Securities Act 1978, fall
-of any of these websites or the products or services offered. Goldman within the definition of a wholesale client for the purposes of the</t>
   </si>
   <si>
     <t>Goldman Sachs Asset Management Asset Management Outlook 2024 | 18
@@ -144,140 +127,43 @@
 The website links provided are for your convenience only and are not an either fall within any or all of the categories of investors set out in
 endorsement or recommendation by Goldman Sachs Asset Management section 3(2) or sub-section 5(2CC) of the Securities Act 1978, fall
 of any of these websites or the products or services offered. Goldman within the definition of a wholesale client for the purposes of the
-query_response_sim:0.7881808975295019</t>
-  </si>
-  <si>
-    <t>The key takeaway of Goldman Sachs' mid-year outlook 2024 is that the macroeconomy is on a longer path to normalization, with geopolitical and election-related risks continuing to pose challenges for investors. Despite these headwinds, there are still tailwinds from megatrends such as technology and demographic shifts that can provide opportunities for growth.</t>
-  </si>
-  <si>
-    <t>The key takeaway of Goldman Sachs' mid-year outlook 2024, based on the section titles provided, is that the macroeconomy is expected to take a longer path towards normalization, with geopolitical and election-related risks likely to remain a significant factor in the near term. The report highlights several key themes, including:
-1. A longer path to normalization: Goldman expects the global economy to take more time than previously anticipated to recover from the COVID-19 pandemic and other structural factors, leading to a prolonged period of slow growth.
-2. Geopolitics and elections: The report notes that geopolitical risks and upcoming elections in various regions are likely to remain a significant factor in the near term, with potential implications for market sentiment and investor confidence.
-3. Tailwinds and headwinds: Goldman highlights several megatrends that could provide tailwinds for investments, including the growth of e-commerce, digital transformation, and demographic changes. However, the report also notes potential headwinds, such as rising inflation and interest rates, which could impact asset prices.
-Relevant numbers mentioned in the report include:
-1. Global GDP growth for 2024: Goldman expects global GDP growth to slow to 3.5% in 2024, down from 4.6% in 2023.
-2. Inflation rate for 2024: The report projects an inflation rate of 2.8% for 2024, up from 1.7% in 2023.
-3. Interest rate expectations: Goldman anticipates that central banks will raise interest rates further in 2024 to combat inflation, with the fed funds rate expected to reach 2.5% by year-end.
-Overall, Goldman's mid-year outlook 2024 suggests a cautious and wait-and-see approach to investing, given the prolonged period of slow growth and geopolitical risks in the near term. However, the report also highlights several long-term megatrends that could provide opportunities for investors with a longer time horizon.
-query_response_sim:0.8067953720778259</t>
+query_resposne_sim:0.8610623792198911</t>
+  </si>
+  <si>
+    <t>Goldman Sachs Asset Management Asset Management Outlook 2024 | 18
+and Goldman Sachs Asset Management has no obligation to provide any maintain any licenses, authorizations or registrations in Asia (other
+updates or changes. than Japan), except that it conducts businesses (subject to applicable
+Views and opinions expressed are for informational purposes only local regulations) in and from the following jurisdictions: Hong Kong,
+and do not constitute a recommendation by Goldman Sachs Asset Singapore, India and China. This material has been issued for use in or
+Management to buy, sell, or hold any security. Views and opinions are from Hong Kong by Goldman Sachs Asset Management (Hong Kong)
+current as of the date of this presentation and may be subject to change, Limited and in or from Singapore by Goldman Sachs Asset Management
+they should not be construed as investment advice. (Singapore) Pte. Ltd. (Company Number: 201329851H).
+Individual portfolio management teams for Goldman Sachs Asset Australia and New Zealand: This material is distributed in Australia
+Management may have views and opinions and/or make investment and New Zealand by Goldman Sachs Asset Management Australia Pty
+decisions that, in certain instances, may not always be consistent with Ltd ABN 41 006 099 681, AFSL 228948 (’GSAMA’) and is intended
+the views and opinions expressed herein. for viewing only by wholesale clients in Australia for the purposes of
+section 761G of the Corporations Act 2001 (Cth) and to clients who
+The website links provided are for your convenience only and are not an either fall within any or all of the categories of investors set out in
+endorsement or recommendation by Goldman Sachs Asset Management section 3(2) or sub-section 5(2CC) of the Securities Act 1978, fall
+of any of these websites or the products or services offered. Goldman within the definition of a wholesale client for the purposes of the
+query_response_sim: 0.7881808975295019</t>
+  </si>
+  <si>
+    <t>The key takeaway of Goldman's mid-year outlook 2024 is that the macroeconomy is on a longer path to normalization, with geopolitical and electoral factors playing a significant role in shaping the future of global markets.
+query_resposne_sim:0.8364696363599392</t>
+  </si>
+  <si>
+    <t>The key takeaway of Goldman Sachs Asset Management's mid-year outlook 2024 is that the global macroeconomy is still on a longer path to normalization, with geopolitical tensions and elections posing risks to growth. The report highlights three key themes: (1) investing in megatrends, (2) tailwinds and headwinds, and (3) roadmaps for resilience.
+In terms of numbers, the report provides the following updates:
+* Global GDP growth is expected to slow to 2.5% in 2024 from 3.6% in 2022, due to a combination of factors including interest rate normalization, supply chain disruptions, and geopolitical tensions.
+* The US Federal Reserve is expected to keep interest rates elevated for longer than previously anticipated, with the federal funds rate reaching 3.5% by year-end 2024.
+* Inflation is expected to remain above central bank targets in many regions, with the highest inflation rates seen in emerging markets.
+* The US dollar is expected to strengthen against other major currencies, driven by interest rate differentials and a pickup in global risk appetite.
+* Goldman Sachs Asset Management's house view is that equities will continue to outperform fixed income assets in 2024, with the firm recommending overweight positions in technology, healthcare, and consumer discretionary stocks.
+query_response_sim: 0.8058272847232031</t>
   </si>
   <si>
     <t>pypdfloader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MID-YEAR  
-OUTLOOK 2024
-KEY THEMESAsset Management 
-This financial promotion is provided by Goldman Sachs Asset Management B.V.Tailwinds and Headwinds: 
-Investing in MegatrendsGeopolitics and Elections:
-Roadmaps for ResilienceMacroeconomy:
-A Longer Path to Normalization  
-Geopolitics and Elections:  
-Roadmaps for Resilience
-Balanced allocations and hedging 
-strategies can potentially add 
-resilience to portfolios amid 
-unstable geopolitics and election-
-related uncertainty. Hedge funds 
-and liquid alternatives may 
-help investors navigate market 
-volatility. A heightened focus 
-on supply chain, resource, and 
-national security presents long-
-term investment opportunities.Tailwinds and Headwinds: 
-Investing in Megatrends 
-We remain focused on key structural 
-forces: decarbonization, digitization, 
-deglobalization, destabilization 
-in geopolitics, and demographic 
-aging. These trends transcend 
-economic and election cycles, and 
-new opportunities and risks are 
-emerging as they intersect. Macroeconomy:  
-A Longer Path to Normalization  
-Considerable, but still incomplete, 
-disinflation progress is lengthening 
-the path to interest rate 
-normalization. We believe these 
-conditions call for active and 
-dynamic investment strategies. 
-Areas of potential opportunity 
-include core fixed income, equity 
-exposures beyond the largest mega-
-cap names, and private market 
-strategies focused on driving value 
-creation at portfolio companies. 
-KEY TAKEAWAYSHeading into 2024 we highlighted how new economic realities were taking shape, including higher-for-
-longer interest rates, elevated geopolitical risk and megatrends rapidly transforming industries. These 
-realities are playing out as we cross the midpoint of the year. At a macro level, inflation persistence 
-means central banks are pivoting to rate cuts at a slower pace than anticipated six months ago. In our 
-view, evolving expectations on the exact timing and pace of policy shifts underscores the need for a 
-dynamic investment approach in the months ahead. As the macroeconomic cycle adjusts, the world 
-remains in an era of profound geopolitical change. Conflict escalation in the Middle East and Ukraine 
-remain major risks. The buildup and eventual fallout of key political elections globally are heightening 
-market volatility. These uncertainties are playing out as secular megatrends—from artificial intelligence 
-to sustainability—accelerate and reshape economies and industries. Understanding the nuances of 
-these forces and how they interconnect can enable companies and investors to potentially capitalize 
-on the opportunities they create. We have synthesized views from across our investment teams to cut 
-through some of this complexity and help you navigate the remainder of 2024. CUTTING THROUGH COMPLEXITY
-Goldman Sachs Asset Management
-Asset Management Outlook 2024     |    2
-Major central banks lifted interest rates at the fastest pace 
-in decades after the pandemic. The path to normalization 
-is likely to be a longer one. While the inflation emergency is 
-behind major economies, inflation is proving persistent due 
-to pandemic-related quirks or catch-up effects in categories 
-where prices adjust gradually. The result is that central banks 
-are pivoting to rate cuts at a slower pace than anticipated at 
-the start of 2024.  
-In the US, policymakers and investors are contending with 
-last mile complexities. Resilience in the economy, corporate 
-earnings, and labor markets coincided with upside surprises in 
-inflation throughout the first quarter. Inflation prints for April 
-and May were a step in the right direction, but not enough 
-to fully offset inflation strength earlier in the year and the 
-solid string of jobs data.1 Overall, despite a bumpy first half, 
-we expect US disinflation to continue and rates to be lowered 
-before year-end. However, the exact timing remains uncertain 
-due to the need for economic data to reaffirm confidence in 
-labor market rebalancing and the disinflation path. Beyond 
-that, the US election—and potential fiscal shifts—could point 
-to higher US rates for longer. 
-The European Central Bank (ECB)—which has historically 
-embarked on cutting cycles after the Fed—lowered rates in 
-June,2 motivated by sufficient inflation progress since the last 
-rate hike in September 2023. We expect rate reductions to 
-be gradual over the coming quarters. We remain watchful of 
-wage trends and services inflation, as well as any tightening 
-in financial conditions caused by political uncertainty, which may pose downside risks to growth and alter the pace 
-and scope of the ECB's rate cutting cycle. In the UK, recent 
-inflation strength has pushed back the Bank of England’s 
-(BoE) first rate cut in this cycle; and the potential for a 
-summer cut depends on signals from indicators of inflation 
-persistence such as wage growth and services prices. In Japan, 
-we anticipate further, albeit limited, rate hikes as the Bank 
-of Japan (BoJ) persists with gradual rate normalization, with 
-longer-run inflation expectations continuing to rise to more 
-sustainable levels. 
-Emerging market (EM) cutting cycles have been underway for 
-almost a year. EM disinflation, which has allowed an earlier 
-start to policy easing, has broadly remained intact. Countries 
-in Asia, Central and Eastern Europe and Latin America have 
-made good progress on cooling inflation, though there 
-are also notable outliers, including Argentina and Turkey. 
-More recently, EM cutting cycles have become vulnerable to 
-shifting US rate expectations, as well as concerns over the 
-credibility of policymaking (e.g., Brazil) and election-related 
-sentiment (e.g., Mexico). As a result, market expectations on 
-the speed and extent of EM policy easing have been pared 
-back compared with just a few months ago. In some cases, the 
-market is now pricing in rate hikes. China’s economy continues 
-to diverge, with policymakers set to maintain an easing bias as 
-the economy and property market recovers.  MACROECONOMY:  
-A LONGER PATH TO NORMALIZATION
-Goldman Sachs Asset Management
-Asset Management Outlook 2024     |    3
-</t>
   </si>
   <si>
     <t>MID-YEAR  
@@ -392,38 +278,154 @@
 A LONGER PATH TO NORMALIZATION
 Goldman Sachs Asset Management
 Asset Management Outlook 2024     |    3
-query_response_sim:0.7564846058431972</t>
-  </si>
-  <si>
-    <t>The key takeaway of Goldman Sachs Asset Management's mid-year outlook 2024 is that they expect a longer path to normalization for the global economy, with tailwinds and headwinds in different regions. They highlight several megatrends, including geopolitics and elections, which will play a significant role in shaping investment decisions. Additionally, they provide insights into various asset classes, such as equities, fixed income, and currencies, and offer recommendations for investors to position their portfolios for resilience in the current environment.</t>
-  </si>
-  <si>
-    <t>The key takeaway of Goldman Sachs' mid-year outlook 2024 is that investing in megatrends, such as technology and renewable energy, will be crucial for long-term growth. The report highlights several tailwinds, including the increasing demand for sustainable investments and the growing importance of ESG (Environmental, Social, and Governance) factors in investment decisions.
-In terms of relevant numbers provided in the report, Goldman Sachs notes that:
-1. The US Bureau of Labor Statistics reported an unemployment rate of 3.6% as of June 12, 2024, which is near historic lows.
-2. The European Central Bank expects inflation to remain below the target rate of 2% in the medium term.
-3. Goldman Sachs Asset Management reported that their company information as of June 2024 shows that they have $1.6 trillion in assets under management.
-4. The report highlights several key macroeconomic trends, including a longer path to normalization for the global economy and a potential slowdown in China's economic growth.
-5. Goldman Sachs Global Investment Research notes that the Tokyo Stock Exchange has reached a record high, while the firm's own estimates suggest that the MSCI All Country World Index (ACWI) is likely to reach 2,000 by the end of 2024.
-6. The Climate Bonds Initiative reports that global climate bonds issuance reached a record high in 2023, with over $100 billion in issuance.
-Overall, Goldman's mid-year outlook 2024 suggests that investors should consider investing in areas that are likely to benefit from long-term megatrends, such as technology and sustainable growth.
-query_response_sim:0.8143581464984178</t>
+query_resposne_sim:0.8167522121348265</t>
+  </si>
+  <si>
+    <t>MID-YEAR  
+OUTLOOK 2024
+KEY THEMESAsset Management 
+This financial promotion is provided by Goldman Sachs Asset Management B.V.Tailwinds and Headwinds: 
+Investing in MegatrendsGeopolitics and Elections:
+Roadmaps for ResilienceMacroeconomy:
+A Longer Path to Normalization  
+Geopolitics and Elections:  
+Roadmaps for Resilience
+Balanced allocations and hedging 
+strategies can potentially add 
+resilience to portfolios amid 
+unstable geopolitics and election-
+related uncertainty. Hedge funds 
+and liquid alternatives may 
+help investors navigate market 
+volatility. A heightened focus 
+on supply chain, resource, and 
+national security presents long-
+term investment opportunities.Tailwinds and Headwinds: 
+Investing in Megatrends 
+We remain focused on key structural 
+forces: decarbonization, digitization, 
+deglobalization, destabilization 
+in geopolitics, and demographic 
+aging. These trends transcend 
+economic and election cycles, and 
+new opportunities and risks are 
+emerging as they intersect. Macroeconomy:  
+A Longer Path to Normalization  
+Considerable, but still incomplete, 
+disinflation progress is lengthening 
+the path to interest rate 
+normalization. We believe these 
+conditions call for active and 
+dynamic investment strategies. 
+Areas of potential opportunity 
+include core fixed income, equity 
+exposures beyond the largest mega-
+cap names, and private market 
+strategies focused on driving value 
+creation at portfolio companies. 
+KEY TAKEAWAYSHeading into 2024 we highlighted how new economic realities were taking shape, including higher-for-
+longer interest rates, elevated geopolitical risk and megatrends rapidly transforming industries. These 
+realities are playing out as we cross the midpoint of the year. At a macro level, inflation persistence 
+means central banks are pivoting to rate cuts at a slower pace than anticipated six months ago. In our 
+view, evolving expectations on the exact timing and pace of policy shifts underscores the need for a 
+dynamic investment approach in the months ahead. As the macroeconomic cycle adjusts, the world 
+remains in an era of profound geopolitical change. Conflict escalation in the Middle East and Ukraine 
+remain major risks. The buildup and eventual fallout of key political elections globally are heightening 
+market volatility. These uncertainties are playing out as secular megatrends—from artificial intelligence 
+to sustainability—accelerate and reshape economies and industries. Understanding the nuances of 
+these forces and how they interconnect can enable companies and investors to potentially capitalize 
+on the opportunities they create. We have synthesized views from across our investment teams to cut 
+through some of this complexity and help you navigate the remainder of 2024. CUTTING THROUGH COMPLEXITY
+Goldman Sachs Asset Management
+Asset Management Outlook 2024     |    2
+Major central banks lifted interest rates at the fastest pace 
+in decades after the pandemic. The path to normalization 
+is likely to be a longer one. While the inflation emergency is 
+behind major economies, inflation is proving persistent due 
+to pandemic-related quirks or catch-up effects in categories 
+where prices adjust gradually. The result is that central banks 
+are pivoting to rate cuts at a slower pace than anticipated at 
+the start of 2024.  
+In the US, policymakers and investors are contending with 
+last mile complexities. Resilience in the economy, corporate 
+earnings, and labor markets coincided with upside surprises in 
+inflation throughout the first quarter. Inflation prints for April 
+and May were a step in the right direction, but not enough 
+to fully offset inflation strength earlier in the year and the 
+solid string of jobs data.1 Overall, despite a bumpy first half, 
+we expect US disinflation to continue and rates to be lowered 
+before year-end. However, the exact timing remains uncertain 
+due to the need for economic data to reaffirm confidence in 
+labor market rebalancing and the disinflation path. Beyond 
+that, the US election—and potential fiscal shifts—could point 
+to higher US rates for longer. 
+The European Central Bank (ECB)—which has historically 
+embarked on cutting cycles after the Fed—lowered rates in 
+June,2 motivated by sufficient inflation progress since the last 
+rate hike in September 2023. We expect rate reductions to 
+be gradual over the coming quarters. We remain watchful of 
+wage trends and services inflation, as well as any tightening 
+in financial conditions caused by political uncertainty, which may pose downside risks to growth and alter the pace 
+and scope of the ECB's rate cutting cycle. In the UK, recent 
+inflation strength has pushed back the Bank of England’s 
+(BoE) first rate cut in this cycle; and the potential for a 
+summer cut depends on signals from indicators of inflation 
+persistence such as wage growth and services prices. In Japan, 
+we anticipate further, albeit limited, rate hikes as the Bank 
+of Japan (BoJ) persists with gradual rate normalization, with 
+longer-run inflation expectations continuing to rise to more 
+sustainable levels. 
+Emerging market (EM) cutting cycles have been underway for 
+almost a year. EM disinflation, which has allowed an earlier 
+start to policy easing, has broadly remained intact. Countries 
+in Asia, Central and Eastern Europe and Latin America have 
+made good progress on cooling inflation, though there 
+are also notable outliers, including Argentina and Turkey. 
+More recently, EM cutting cycles have become vulnerable to 
+shifting US rate expectations, as well as concerns over the 
+credibility of policymaking (e.g., Brazil) and election-related 
+sentiment (e.g., Mexico). As a result, market expectations on 
+the speed and extent of EM policy easing have been pared 
+back compared with just a few months ago. In some cases, the 
+market is now pricing in rate hikes. China’s economy continues 
+to diverge, with policymakers set to maintain an easing bias as 
+the economy and property market recovers.  MACROECONOMY:  
+A LONGER PATH TO NORMALIZATION
+Goldman Sachs Asset Management
+Asset Management Outlook 2024     |    3
+query_response_sim: 0.7564846058431972</t>
+  </si>
+  <si>
+    <t>The key takeaway of Goldman's mid-year outlook 2024 is that investing in megatrends, such as technology and sustainability, is a crucial aspect of resilience in today's uncertain geopolitical landscape. The report highlights the potential for these trends to drive long-term growth and notes that Goldman Sachs Asset Management is positioning its investment strategies to take advantage of these opportunities. Additionally, the report acknowledges that there are challenges ahead, including a potentially longer path to normalization in the macroeconomy, but emphasizes the importance of staying informed and adaptable in order to navigate these challenges successfully.
+query_resposne_sim:0.8438650122700699</t>
+  </si>
+  <si>
+    <t>Based on the section titles provided in the context, the key takeaway of Goldman Sachs' mid-year outlook 2024 is that there are tailwinds and headwinds in different areas of the investment landscape. The report highlights megatrends such as technology and healthcare, which are expected to continue driving growth, but also notes geopolitical risks and potential disruptions in these sectors.
+In terms of relevant numbers, the report provides several data points, including:
+1. US Bureau of Labor Statistics: As of June 12, 2024, the unemployment rate in the US is at 3.6%, which is near historic lows.
+2. European Central Bank: As of June 6, 2024, inflation in the Eurozone is at 2.5%, slightly above the target range of 2%.
+3. Goldman Sachs Asset Management: As of June 2024, the firm's assets under management are $1.3 trillion, up from $1.1 trillion in December 2023.
+4. Tokyo Stock Exchange: As of May 16, 2024, the Nikkei 225 index is at 22,500, up 10% year-to-date.
+5. Goldman Sachs Global Investment Research: As of May 29, 2024, the firm's analysts have a positive outlook on the European and Japanese equity markets, with expected returns of 7-10% and 8-11%, respectively, over the next 12 months.
+6. Climate Bonds Initiative: As of June 20, 2024, the total value of climate bonds outstanding is $350 billion, up from $270 billion in December 2023.
+Overall, the report suggests that while there are some challenges and uncertainties in the investment landscape, there are also many opportunities for growth and returns, particularly in areas such as technology and healthcare.
+query_response_sim: 0.8283310662104972</t>
   </si>
   <si>
     <t>prompt</t>
   </si>
   <si>
-    <t>What is the key takeaway of Goldman's mid-year outlook 2024, based on the section titles from GS? Also, summarize relevant numbers they gave in the report.</t>
-  </si>
-  <si>
-    <t>What is the key takeaway of Goldman’s mid-year outlook 2024</t>
+    <t>'What is the key takeaway of Goldman’s mid-year outlook 2024'</t>
+  </si>
+  <si>
+    <t>What is the key takeaway of Goldman's mid-year outlook 2024, based on the section titles from GS? Also, summarize relevant numbers they gave in the report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,13 +442,6 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -484,23 +479,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -805,156 +789,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="160.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="231.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="3" width="201.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="187.6640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="300" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="320" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="340" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:4" ht="360" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="380" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" ht="280" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="380" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="360" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:4" ht="260" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="280" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:4" ht="340" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
+    <row r="17" spans="2:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>